<commit_message>
feat: Update budget reader to handle DataFrame and dict types; modify settings for column naming consistency
</commit_message>
<xml_diff>
--- a/data/orcamentos/sample_padrao1.xlsx
+++ b/data/orcamentos/sample_padrao1.xlsx
@@ -373,10 +373,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -789,7 +785,7 @@
   <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: Implement value conversion utility and update budget reader for type handling
</commit_message>
<xml_diff>
--- a/data/orcamentos/sample_padrao1.xlsx
+++ b/data/orcamentos/sample_padrao1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/orcamentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="11_2B5A8FE7125C5C426140C57430267256DF8CDB53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A4E47CF-0496-42E1-A10D-6528045B5190}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="11_2B5A8FE7125C5C426140C57430267256DF8CDB53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A85B09BB-2040-4EBD-AF14-2B5B99E8974A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="66">
   <si>
     <t>ITAÚ UNIBANCO S/A - Ag. 4830 - SANTOS - BOQUEIRÃO - SP</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Quant</t>
+  </si>
+  <si>
+    <t>UPE</t>
   </si>
 </sst>
 </file>
@@ -373,6 +376,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -662,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,6 +736,12 @@
       </c>
       <c r="H5" t="s">
         <v>61</v>
+      </c>
+      <c r="K5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5">
+        <v>188292</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -784,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>